<commit_message>
fin de l'implémentation du header (filtres, infos recherche)
</commit_message>
<xml_diff>
--- a/documents/tableau de bord/journal de bord.xlsx
+++ b/documents/tableau de bord/journal de bord.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>projet</t>
   </si>
@@ -94,13 +94,37 @@
   </si>
   <si>
     <t>pratique délibérée</t>
+  </si>
+  <si>
+    <t>Intégration du HEADER et du FOOTER</t>
+  </si>
+  <si>
+    <t>RAS</t>
+  </si>
+  <si>
+    <t>AGENCEMENT DU NAV</t>
+  </si>
+  <si>
+    <t>REGROUPEMENT DU MENU ET INSCRIPTION DANS UNE DIV + FLEXBOX</t>
+  </si>
+  <si>
+    <t>FUSION DES ELEMENTS DE LA BARRE DE RECHERCHE</t>
+  </si>
+  <si>
+    <t>RESERVIA VERSION DESKTOP</t>
+  </si>
+  <si>
+    <t>Solutions</t>
+  </si>
+  <si>
+    <t>FLEXBOX ROW FLEX-START+ PADDING NEGATIF + Z-INDEX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,16 +132,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -125,16 +171,195 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,10 +654,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -442,291 +670,381 @@
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="39.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="21">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="B1" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="21">
+      <c r="A2" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="45">
-      <c r="A5" s="1" t="s">
+      <c r="B2" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="63">
+      <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
+      <c r="K5" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>44253</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>44253</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>2</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <f>F6*30</f>
         <v>60</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>2</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <f>H6*30</f>
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
+      <c r="J6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>44253</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>44253</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <f t="shared" ref="G7:G14" si="0">F7*30</f>
         <v>30</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>1</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <f t="shared" ref="I7:I14" si="1">H7*30</f>
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
+      <c r="J7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="13"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>44253</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>44253</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>1</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>1</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
+      <c r="J8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="1:11" ht="30">
+      <c r="A9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
+        <v>44255</v>
+      </c>
+      <c r="E9" s="3">
+        <v>44255</v>
+      </c>
+      <c r="F9" s="2">
+        <v>3</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="H9" s="2">
+        <v>2</v>
+      </c>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3">
         <v>44254</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E10" s="3">
         <v>44254</v>
       </c>
-      <c r="G9">
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I9">
+        <v>30</v>
+      </c>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="1:11" ht="45">
+      <c r="A11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3">
+        <v>44255</v>
+      </c>
+      <c r="E11" s="3">
+        <v>44255</v>
+      </c>
+      <c r="F11" s="2">
+        <v>3</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3">
+        <v>44256</v>
+      </c>
+      <c r="E12" s="3">
+        <v>44256</v>
+      </c>
+      <c r="F12" s="2">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2</v>
+      </c>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3">
+        <v>44256</v>
+      </c>
+      <c r="E13" s="3">
+        <v>44256</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H13" s="2">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+    </row>
+    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="10">
+        <v>44257</v>
+      </c>
+      <c r="E14" s="10">
+        <v>44257</v>
+      </c>
+      <c r="F14" s="9">
+        <v>1</v>
+      </c>
+      <c r="G14" s="9">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
+      <c r="J14" s="14"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+      <c r="F15" s="17">
+        <f>SUM(F6:F14)</f>
         <v>16</v>
       </c>
-      <c r="B10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="2">
-        <v>44254</v>
-      </c>
-      <c r="E10" s="2">
-        <v>44254</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2">
-        <v>44255</v>
-      </c>
-      <c r="E11" s="2">
-        <v>44255</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2">
-        <v>44256</v>
-      </c>
-      <c r="E12" s="2">
-        <v>44256</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="2">
-        <v>44256</v>
-      </c>
-      <c r="E13" s="2">
-        <v>44256</v>
-      </c>
-      <c r="G13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="2">
-        <v>44257</v>
-      </c>
-      <c r="E14" s="2">
-        <v>44257</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G15" s="16">
+        <f>SUM(G6:G14)</f>
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -745,6 +1063,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
intégration du footer, préparation intégration du Hosting
</commit_message>
<xml_diff>
--- a/documents/tableau de bord/journal de bord.xlsx
+++ b/documents/tableau de bord/journal de bord.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="étape 1" sheetId="1" r:id="rId1"/>
+    <sheet name="étape 2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
   <si>
     <t>projet</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>FLEXBOX ROW FLEX-START+ PADDING NEGATIF + Z-INDEX</t>
+  </si>
+  <si>
+    <t>travail réel      (cycle Podomoro)</t>
+  </si>
+  <si>
+    <t>Intégration de la partie HOSTING</t>
   </si>
 </sst>
 </file>
@@ -163,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -321,11 +327,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -360,6 +379,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,11 +676,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
+      <selection pane="bottomRight" sqref="A1:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -970,7 +990,9 @@
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
-      <c r="J12" s="12"/>
+      <c r="J12" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="K12" s="13"/>
     </row>
     <row r="13" spans="1:11">
@@ -1003,7 +1025,9 @@
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J13" s="12"/>
+      <c r="J13" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="K13" s="13"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1">
@@ -1020,7 +1044,7 @@
         <v>44257</v>
       </c>
       <c r="E14" s="10">
-        <v>44257</v>
+        <v>44258</v>
       </c>
       <c r="F14" s="9">
         <v>1</v>
@@ -1029,12 +1053,16 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H14" s="9"/>
+      <c r="H14" s="9">
+        <v>1</v>
+      </c>
       <c r="I14" s="9">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="14"/>
+        <v>30</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>27</v>
+      </c>
       <c r="K14" s="15"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1">
@@ -1045,6 +1073,14 @@
       <c r="G15" s="16">
         <f>SUM(G6:G14)</f>
         <v>480</v>
+      </c>
+      <c r="H15" s="17">
+        <f>SUM(H6:H14)</f>
+        <v>13</v>
+      </c>
+      <c r="I15" s="18">
+        <f>SUM(I6:I14)</f>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -1069,12 +1105,320 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" customWidth="1"/>
+    <col min="11" max="11" width="29.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="21">
+      <c r="A1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="21">
+      <c r="A2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="15.75" thickBot="1"/>
+    <row r="5" spans="1:11" ht="47.25">
+      <c r="A5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="7"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <f>F6*30</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2">
+        <f>H6*30</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="13"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="7"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <f t="shared" ref="G7:G16" si="0">F7*30</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2">
+        <f t="shared" ref="I7:I16" si="1">H7*30</f>
+        <v>0</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="13"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="7"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="12"/>
+      <c r="K8" s="13"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="7"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="12"/>
+      <c r="K9" s="13"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="7"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="12"/>
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="7"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="12"/>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="7"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="7"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="12"/>
+      <c r="K13" s="13"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="7"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="12"/>
+      <c r="K14" s="13"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="7"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="K15" s="13"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="9"/>
+      <c r="I16" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="14"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="6:9" ht="15.75" thickBot="1">
+      <c r="F17" s="17">
+        <f>SUM(F6:F16)</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="16">
+        <f>SUM(G6:G16)</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="17">
+        <f>SUM(H6:H16)</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="18">
+        <f>SUM(I6:I16)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H16 F6:F16">
+      <formula1>"0,1,2,3,4,5,6"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:E16">
+      <formula1>"04-mars, 05-mars, 06-mars, 07-mars, 08-mars"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C16">
+      <formula1>"activité complémentaire,séance guidée,pratique délibérée"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B16">
+      <formula1>"openclassrooms,mission,autres"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
intégration des cartes du block les plus populaires
</commit_message>
<xml_diff>
--- a/documents/tableau de bord/journal de bord.xlsx
+++ b/documents/tableau de bord/journal de bord.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
   <si>
     <t>projet</t>
   </si>
@@ -124,6 +124,21 @@
   </si>
   <si>
     <t>Intégration de la partie HOSTING</t>
+  </si>
+  <si>
+    <t>intégration du titre du block most_pop_hosting</t>
+  </si>
+  <si>
+    <t>intégration des cartes du block most_pop_hosting</t>
+  </si>
+  <si>
+    <t>intégration du titre du block hosting</t>
+  </si>
+  <si>
+    <t>intégration des cartes du block hosting</t>
+  </si>
+  <si>
+    <t>flex froggy</t>
   </si>
 </sst>
 </file>
@@ -680,7 +695,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:K15"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1108,12 +1123,12 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H9" sqref="H8:H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.140625" customWidth="1"/>
     <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -1178,53 +1193,93 @@
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="7"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
+      <c r="A6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3">
+        <v>44259</v>
+      </c>
+      <c r="E6" s="3">
+        <v>44259</v>
+      </c>
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
       <c r="G6" s="2">
         <f>F6*30</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
       <c r="I6" s="2">
         <f>H6*30</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J6" s="12"/>
       <c r="K6" s="13"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="7"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="2"/>
+      <c r="A7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3">
+        <v>44260</v>
+      </c>
+      <c r="E7" s="3">
+        <v>44261</v>
+      </c>
+      <c r="F7" s="2">
+        <v>6</v>
+      </c>
       <c r="G7" s="2">
         <f t="shared" ref="G7:G16" si="0">F7*30</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="2"/>
+        <v>180</v>
+      </c>
+      <c r="H7" s="2">
+        <v>4</v>
+      </c>
       <c r="I7" s="2">
         <f t="shared" ref="I7:I16" si="1">H7*30</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="J7" s="12"/>
       <c r="K7" s="13"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="7"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="2"/>
+      <c r="A8" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3">
+        <v>44261</v>
+      </c>
+      <c r="E8" s="3">
+        <v>44261</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
       <c r="G8" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2">
@@ -1235,15 +1290,27 @@
       <c r="K8" s="13"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="7"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="2"/>
+      <c r="A9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3">
+        <v>44262</v>
+      </c>
+      <c r="E9" s="3">
+        <v>44263</v>
+      </c>
+      <c r="F9" s="2">
+        <v>6</v>
+      </c>
       <c r="G9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2">
@@ -1254,15 +1321,27 @@
       <c r="K9" s="13"/>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="7"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="2"/>
+      <c r="A10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3">
+        <v>44259</v>
+      </c>
+      <c r="E10" s="3">
+        <v>44259</v>
+      </c>
+      <c r="F10" s="2">
+        <v>1</v>
+      </c>
       <c r="G10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2">
@@ -1389,19 +1468,19 @@
     <row r="17" spans="6:9" ht="15.75" thickBot="1">
       <c r="F17" s="17">
         <f>SUM(F6:F16)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="G17" s="16">
         <f>SUM(G6:G16)</f>
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="H17" s="17">
         <f>SUM(H6:H16)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I17" s="18">
         <f>SUM(I6:I16)</f>
-        <v>0</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise à jour du tableau de bord
</commit_message>
<xml_diff>
--- a/documents/tableau de bord/journal de bord.xlsx
+++ b/documents/tableau de bord/journal de bord.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
   <si>
     <t>projet</t>
   </si>
@@ -139,6 +139,18 @@
   </si>
   <si>
     <t>flex froggy</t>
+  </si>
+  <si>
+    <t>largeur des cartes, div image qui sortait de la largeur de la carte</t>
+  </si>
+  <si>
+    <t>largeur des cartes fixée à 30% de l'espace hébergement, largeur div image en mode auto</t>
+  </si>
+  <si>
+    <t>réaliser une card css</t>
+  </si>
+  <si>
+    <t>autres</t>
   </si>
 </sst>
 </file>
@@ -1120,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H8:H9"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1245,14 +1257,14 @@
         <v>6</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ref="G7:G16" si="0">F7*30</f>
+        <f t="shared" ref="G7:G11" si="0">F7*30</f>
         <v>180</v>
       </c>
       <c r="H7" s="2">
         <v>4</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" ref="I7:I16" si="1">H7*30</f>
+        <f t="shared" ref="I7:I11" si="1">H7*30</f>
         <v>120</v>
       </c>
       <c r="J7" s="12"/>
@@ -1281,15 +1293,17 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
       <c r="I8" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J8" s="12"/>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" ht="60">
       <c r="A9" s="7" t="s">
         <v>39</v>
       </c>
@@ -1312,13 +1326,19 @@
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>5</v>
+      </c>
       <c r="I9" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J9" s="12"/>
-      <c r="K9" s="13"/>
+        <v>150</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="7" t="s">
@@ -1343,158 +1363,79 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <v>1</v>
+      </c>
       <c r="I10" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J10" s="12"/>
       <c r="K10" s="13"/>
     </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="7"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="2"/>
+    <row r="11" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A11" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="3">
+        <v>44261</v>
+      </c>
+      <c r="E11" s="3">
+        <v>44261</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
       <c r="G11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H11" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
       <c r="I11" s="2">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="J11" s="12"/>
       <c r="K11" s="13"/>
     </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="7"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="13"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="7"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="13"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="7"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="13"/>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="7"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="9"/>
-      <c r="I16" s="2">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="17" spans="6:9" ht="15.75" thickBot="1">
-      <c r="F17" s="17">
-        <f>SUM(F6:F16)</f>
-        <v>15</v>
-      </c>
-      <c r="G17" s="16">
-        <f>SUM(G6:G16)</f>
-        <v>450</v>
-      </c>
-      <c r="H17" s="17">
-        <f>SUM(H6:H16)</f>
-        <v>5</v>
-      </c>
-      <c r="I17" s="18">
-        <f>SUM(I6:I16)</f>
-        <v>150</v>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1">
+      <c r="F12" s="17">
+        <f>SUM(F6:F11)</f>
+        <v>16</v>
+      </c>
+      <c r="G12" s="16">
+        <f>SUM(G6:G11)</f>
+        <v>480</v>
+      </c>
+      <c r="H12" s="17">
+        <f>SUM(H6:H11)</f>
+        <v>13</v>
+      </c>
+      <c r="I12" s="18">
+        <f>SUM(I6:I11)</f>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H16 F6:F16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H11 F6:F11">
       <formula1>"0,1,2,3,4,5,6"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:E16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:E11">
       <formula1>"04-mars, 05-mars, 06-mars, 07-mars, 08-mars"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C6:C11">
       <formula1>"activité complémentaire,séance guidée,pratique délibérée"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6:B11">
       <formula1>"openclassrooms,mission,autres"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
intégration de la partie activité réservia
</commit_message>
<xml_diff>
--- a/documents/tableau de bord/journal de bord.xlsx
+++ b/documents/tableau de bord/journal de bord.xlsx
@@ -1135,7 +1135,7 @@
   <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1345,10 +1345,10 @@
         <v>40</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3">
         <v>44259</v>

</xml_diff>